<commit_message>
Basic Attacks and abilities
Buttons have stopped working and floats arent working in the pet class
</commit_message>
<xml_diff>
--- a/Battle Pets/Assets/Data/PetSheet.xlsx
+++ b/Battle Pets/Assets/Data/PetSheet.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\GAM111 - Battle Pets\BattlePets\Assets\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\GitHub\BattlePets\Battle Pets\Assets\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -59,18 +59,6 @@
     <t>AirRes</t>
   </si>
   <si>
-    <t>FireBird</t>
-  </si>
-  <si>
-    <t>WaterFish</t>
-  </si>
-  <si>
-    <t>RockLizard</t>
-  </si>
-  <si>
-    <t>AirSnail</t>
-  </si>
-  <si>
     <t>Air</t>
   </si>
   <si>
@@ -81,6 +69,30 @@
   </si>
   <si>
     <t>Fire</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>Levithan</t>
+  </si>
+  <si>
+    <t>Golem</t>
+  </si>
+  <si>
+    <t>Solid Storm</t>
+  </si>
+  <si>
+    <t>Water Fish</t>
+  </si>
+  <si>
+    <t>Rock Lizard</t>
+  </si>
+  <si>
+    <t>Fire Bird</t>
+  </si>
+  <si>
+    <t>Air Snail</t>
   </si>
 </sst>
 </file>
@@ -398,10 +410,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -448,10 +460,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C2">
         <v>60</v>
@@ -483,10 +495,10 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C3">
         <v>50</v>
@@ -518,10 +530,10 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4">
         <v>80</v>
@@ -553,10 +565,10 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C5">
         <v>30</v>
@@ -583,6 +595,146 @@
         <v>40</v>
       </c>
       <c r="K5">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>45</v>
+      </c>
+      <c r="D6">
+        <v>8</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>80</v>
+      </c>
+      <c r="I6">
+        <v>40</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>33</v>
+      </c>
+      <c r="D7">
+        <v>4</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>20</v>
+      </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7">
+        <v>100</v>
+      </c>
+      <c r="K7">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>65</v>
+      </c>
+      <c r="D8">
+        <v>5</v>
+      </c>
+      <c r="E8">
+        <v>7</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>60</v>
+      </c>
+      <c r="I8">
+        <v>80</v>
+      </c>
+      <c r="J8">
+        <v>40</v>
+      </c>
+      <c r="K8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>4</v>
+      </c>
+      <c r="E9">
+        <v>3</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>40</v>
+      </c>
+      <c r="I9">
+        <v>40</v>
+      </c>
+      <c r="J9">
+        <v>40</v>
+      </c>
+      <c r="K9">
         <v>80</v>
       </c>
     </row>

</xml_diff>